<commit_message>
feat(requirements): add data flow
</commit_message>
<xml_diff>
--- a/presentations/pal2_tabelle.xlsx
+++ b/presentations/pal2_tabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuebra.tokuc/workspace/bachelor-thesis/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790EFDD-C726-CC4C-8883-35D04B76CCBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D5C351-122B-CD4E-A68D-883A8CAD8980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72000" yWindow="-10200" windowWidth="38400" windowHeight="21600" xr2:uid="{CB294B4E-8884-5F45-AE87-A799F34C1F90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CB294B4E-8884-5F45-AE87-A799F34C1F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="150">
   <si>
     <t>Gesamtsystem</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Einflussfaktor/Quelle/Notiz</t>
   </si>
   <si>
-    <t>Anlagen müssen kommunikationsfähig sein</t>
-  </si>
-  <si>
     <t>Dezentrale Energieerzeugung erfordert Koordination der Informationen für Einspeisung in das Netz</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Anlagen in ein IoT-Netzwerk integrieren</t>
   </si>
   <si>
-    <t>Anlagen müssen ihren Zustand/ ihre Umgebung melden können</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leistungsqualität und Hohe Verfügbarkeit der Leistung muss gewährleistet werden </t>
   </si>
   <si>
@@ -122,12 +116,6 @@
     <t>technische Ebene</t>
   </si>
   <si>
-    <t xml:space="preserve">Cloud-Applikation zur Zustandsüberwachung </t>
-  </si>
-  <si>
-    <t>Ständige Verfügbarkeit von Informationen in Echtzeit</t>
-  </si>
-  <si>
     <t>R: Referenzarchitektur für standardisiertes Vorgehen benötigt</t>
   </si>
   <si>
@@ -191,9 +179,6 @@
     <t>R: SAP Leonardo Schnittstellen</t>
   </si>
   <si>
-    <t>R: SAP Cloud Platform</t>
-  </si>
-  <si>
     <t xml:space="preserve">F: generiere Alerts </t>
   </si>
   <si>
@@ -272,9 +257,6 @@
     <t>klingt kacke getrennt</t>
   </si>
   <si>
-    <t>Simulation einer realen Anlage</t>
-  </si>
-  <si>
     <t>Rasberry Pi 3</t>
   </si>
   <si>
@@ -344,9 +326,6 @@
     <t>F: Die Hardware muss fähig sein, REST-Daten über eine Web API zu verschicken</t>
   </si>
   <si>
-    <t>F: Die Hardware muss eine Verbindung zum Internet haben</t>
-  </si>
-  <si>
     <t xml:space="preserve">F: Das Edge-Gerät kann fähig sein, die Messwerte vor dem Versenden aufzubereiten </t>
   </si>
   <si>
@@ -474,6 +453,36 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Anlagen müssen ihren Zustand/ ihre Umgebung in Echtzeit melden können</t>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Cloud-Applikation) zur Zustandsüberwachung </t>
+  </si>
+  <si>
+    <t>Anlagen müssen kommunikationsfähig sein/Digitaler Zwilling</t>
+  </si>
+  <si>
+    <t>Ständige Verfügbarkeit von Informationen in Echtzeit unabhängig vom Ort</t>
+  </si>
+  <si>
+    <t>F: Die Hardware muss netzwerkfähig sein</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikation der Werte an zentrale Stelle </t>
+  </si>
+  <si>
+    <t>R: Cloud</t>
+  </si>
+  <si>
+    <t>Simulation einer realen Anlage/ Erzeugung eines cyber-physischen Systems als Messinstrument</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,21 +621,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -640,9 +634,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -662,6 +653,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,14 +991,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0C582B-7A07-3644-9B2B-84054A20C597}">
   <dimension ref="A2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="70.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" style="17" customWidth="1"/>
+    <col min="2" max="2" width="53" style="11" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
@@ -994,18 +1006,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1016,639 +1028,663 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="34">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34">
-      <c r="A7" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="17" t="s">
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="31" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="41" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
+      <c r="E11" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>31</v>
+      <c r="B12" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17">
       <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34">
-      <c r="B14" s="17" t="s">
-        <v>113</v>
+      <c r="B14" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34">
+      <c r="B15" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="68">
+      <c r="B16" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34">
-      <c r="B15" s="17" t="s">
+    <row r="18" spans="1:5">
+      <c r="E18" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="68">
-      <c r="B16" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="E18" s="12" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="E19" s="19" t="s">
-        <v>143</v>
+      <c r="E19" s="13" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="E20" s="20" t="s">
-        <v>144</v>
+      <c r="E20" s="14" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="33" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>108</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="17">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17">
+      <c r="A24" s="20"/>
+      <c r="B24" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17">
+      <c r="A25" s="20"/>
+      <c r="B25" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17">
+      <c r="A26" s="20"/>
+      <c r="B26" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17">
-      <c r="A24" s="4"/>
-      <c r="B24" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17">
-      <c r="A25" s="4"/>
-      <c r="B25" s="17" t="s">
+    </row>
+    <row r="27" spans="1:5" ht="34">
+      <c r="B27" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="17">
-      <c r="A26" s="4"/>
-      <c r="B26" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="34">
-      <c r="B27" s="17" t="s">
-        <v>95</v>
+      <c r="D27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="34">
-      <c r="B28" s="17" t="s">
-        <v>96</v>
+      <c r="B28" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="29" customHeight="1">
-      <c r="B29" s="17" t="s">
-        <v>97</v>
+      <c r="B29" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34">
-      <c r="B30" s="17" t="s">
-        <v>108</v>
+      <c r="B30" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="34">
+      <c r="B35" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="68">
+      <c r="B36" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
         <v>105</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="34">
-      <c r="B35" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="68">
-      <c r="B36" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" ht="34">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="34">
+      <c r="A39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="34">
+      <c r="A40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17">
+      <c r="A41" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="34">
+      <c r="A42" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="13" t="s">
+      <c r="C42" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="34">
-      <c r="A39" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" s="15"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:5" ht="34">
+      <c r="A44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17">
+      <c r="A45" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="34">
-      <c r="A40" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17">
-      <c r="A41" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="34">
-      <c r="A42" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="21"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="13"/>
-    </row>
-    <row r="44" spans="1:5" ht="34">
-      <c r="A44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="17">
-      <c r="A45" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="51">
       <c r="A46" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17">
       <c r="A47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17">
-      <c r="B48" s="17" t="s">
-        <v>120</v>
+      <c r="B48" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="34">
       <c r="A49" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+    </row>
+    <row r="52" spans="1:4" ht="34">
+      <c r="B52" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="34">
+      <c r="B53" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="51">
+      <c r="B54" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="34">
+      <c r="B55" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17">
+      <c r="B56" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17">
+      <c r="B57" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1">
+      <c r="B58" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="1:4" ht="34">
-      <c r="B52" s="17" t="s">
+      <c r="C58" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1">
+      <c r="B59" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="34">
-      <c r="B53" s="17" t="s">
+      <c r="C59" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1">
+      <c r="B60" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="51">
-      <c r="B54" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="34">
-      <c r="B55" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="17">
-      <c r="B56" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="17">
-      <c r="B57" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1">
-      <c r="B58" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1">
-      <c r="B59" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1">
-      <c r="B60" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1"/>
     <row r="62" spans="1:4" ht="15" customHeight="1"/>
     <row r="63" spans="1:4">
-      <c r="A63" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+      <c r="A63" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
     </row>
     <row r="65" spans="1:5" ht="17">
-      <c r="B65" s="17" t="s">
-        <v>52</v>
+      <c r="A65" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17">
-      <c r="B66" s="17" t="s">
-        <v>51</v>
+      <c r="B66" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17">
-      <c r="B67" s="17" t="s">
-        <v>53</v>
+      <c r="B67" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="34">
       <c r="A68" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>98</v>
+        <v>149</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="9" t="s">
-        <v>106</v>
+      <c r="D68" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17">
       <c r="A69" s="3"/>
-      <c r="B69" s="17" t="s">
-        <v>99</v>
+      <c r="B69" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="9"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:5" ht="17">
       <c r="A70" s="3"/>
-      <c r="B70" s="17" t="s">
-        <v>100</v>
+      <c r="B70" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="9"/>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:5" ht="17">
       <c r="A71" s="3"/>
-      <c r="B71" s="17" t="s">
-        <v>101</v>
+      <c r="B71" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="9"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:5" ht="34">
       <c r="A72" s="3"/>
-      <c r="B72" s="17" t="s">
-        <v>102</v>
+      <c r="B72" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C72" s="3"/>
-      <c r="D72" s="9" t="s">
-        <v>107</v>
+      <c r="D72" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17">
       <c r="A73" s="3"/>
-      <c r="B73" s="17" t="s">
-        <v>103</v>
+      <c r="B73" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="C73" s="3"/>
-      <c r="D73" s="9"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="34">
       <c r="A74" s="3"/>
-      <c r="B74" s="17" t="s">
-        <v>104</v>
+      <c r="B74" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="9"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:5" ht="34">
       <c r="A75" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D75" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="34">
       <c r="A76" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="34">
       <c r="A77" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="17" t="s">
         <v>64</v>
       </c>
+      <c r="B77" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D77" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E77" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="17">
       <c r="A78" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>66</v>
+        <v>33</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="17">
       <c r="A79" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>